<commit_message>
Adds a bit of i18n
</commit_message>
<xml_diff>
--- a/examples/input/test_model.xlsx
+++ b/examples/input/test_model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\neural_network\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\neural_network\train\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA6AE91-8CD2-41F0-B224-B1E1A12C120E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D16BB6E-BFF2-473F-8D50-8DD4DDFDE487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,12 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>sig(0.90)</t>
   </si>
   <si>
     <t>lin(0.70)</t>
+  </si>
+  <si>
+    <t>Коэффициент скорости обучения</t>
+  </si>
+  <si>
+    <t>Количество входов нейронной сети</t>
+  </si>
+  <si>
+    <t>Размерность выходного слоя</t>
   </si>
 </sst>
 </file>
@@ -379,24 +388,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1">
         <v>0.9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
-      <c r="B2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
     </row>

</xml_diff>